<commit_message>
update Project Track.xlsx status.
</commit_message>
<xml_diff>
--- a/schedule/Project Track.xlsx
+++ b/schedule/Project Track.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Port Plan" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="88">
   <si>
     <t>Decription</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,10 +227,6 @@
     <t>Processing</t>
   </si>
   <si>
-    <t>Processing</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Iterate</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -251,10 +247,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>vpi_delay</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>vpi_arrayvalue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -304,6 +296,154 @@
   </si>
   <si>
     <t>Data Structure</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vpi_handle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vpi_delays</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Use tuple store delays.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vpi_vector</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Need change value from list to tuple.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The free function embedded in vpiHandle object.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid</t>
+  </si>
+  <si>
+    <t>Status</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>This function can be applied to all objects with</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a fullname property</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When scope is NULL,
+The function will return a right handle with a right hierarchy full name, and will search within that scope if scope is supported.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>When access a protected scope object, an error will occur.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>The VPI routine</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> vpi_handle_by_index() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">shall return a handle to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">an object based on the index number of the object within the reference object, obj. </t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Access a object without a legal SystemVerilog index select object, Null will return.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Access an array element successful.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Access a vector bit successful.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Points Decription</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Test Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -311,7 +451,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,16 +501,62 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -378,21 +564,104 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="43">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF339933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -417,6 +686,20 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF339933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -445,6 +728,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -466,6 +756,27 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF339933"/>
         </patternFill>
       </fill>
@@ -473,6 +784,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -501,6 +819,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -529,6 +854,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -550,6 +882,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF339933"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -571,7 +910,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF339933"/>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
     </dxf>
@@ -585,6 +924,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
@@ -592,28 +938,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -912,10 +1244,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -926,35 +1261,35 @@
     <col min="4" max="4" width="51" customWidth="1"/>
     <col min="5" max="5" width="18.25" customWidth="1"/>
     <col min="6" max="6" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="18.625" customWidth="1"/>
+    <col min="7" max="7" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="20.25">
-      <c r="A1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="3" t="s">
+    <row r="1" spans="1:7" s="3" customFormat="1" ht="21" thickBot="1">
+      <c r="A1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="14.25">
       <c r="A2" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1028,7 +1363,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
@@ -1042,7 +1377,7 @@
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
@@ -1056,7 +1391,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E9" t="s">
         <v>43</v>
@@ -1070,7 +1405,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
@@ -1084,7 +1419,7 @@
         <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
@@ -1098,10 +1433,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F12" t="s">
         <v>2</v>
@@ -1112,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F13" t="s">
         <v>2</v>
@@ -1151,7 +1486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:6" outlineLevel="1">
+    <row r="17" spans="2:7" outlineLevel="1">
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -1162,7 +1497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="2:6" outlineLevel="1">
+    <row r="18" spans="2:7" outlineLevel="1">
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -1173,7 +1508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="2:6" outlineLevel="1">
+    <row r="19" spans="2:7" outlineLevel="1">
       <c r="B19" t="s">
         <v>18</v>
       </c>
@@ -1184,7 +1519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:6" outlineLevel="1">
+    <row r="20" spans="2:7" outlineLevel="1">
       <c r="B20" t="s">
         <v>19</v>
       </c>
@@ -1195,7 +1530,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="2:6" outlineLevel="1">
+    <row r="21" spans="2:7" outlineLevel="1">
       <c r="B21" t="s">
         <v>20</v>
       </c>
@@ -1206,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="2:6" outlineLevel="1">
+    <row r="22" spans="2:7" outlineLevel="1">
       <c r="B22" t="s">
         <v>21</v>
       </c>
@@ -1217,7 +1552,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="2:6" outlineLevel="1">
+    <row r="23" spans="2:7" outlineLevel="1">
       <c r="B23" t="s">
         <v>22</v>
       </c>
@@ -1228,7 +1563,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="2:6" outlineLevel="1">
+    <row r="24" spans="2:7" outlineLevel="1">
       <c r="B24" t="s">
         <v>23</v>
       </c>
@@ -1239,7 +1574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:6" outlineLevel="1">
+    <row r="25" spans="2:7" outlineLevel="1">
       <c r="B25" t="s">
         <v>24</v>
       </c>
@@ -1250,7 +1585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:6" outlineLevel="1">
+    <row r="26" spans="2:7" outlineLevel="1">
       <c r="B26" t="s">
         <v>25</v>
       </c>
@@ -1261,7 +1596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:6" outlineLevel="1">
+    <row r="27" spans="2:7" outlineLevel="1">
       <c r="B27" t="s">
         <v>26</v>
       </c>
@@ -1272,7 +1607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="2:6" outlineLevel="1">
+    <row r="28" spans="2:7" outlineLevel="1">
       <c r="B28" t="s">
         <v>27</v>
       </c>
@@ -1283,7 +1618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:6" outlineLevel="1">
+    <row r="29" spans="2:7" outlineLevel="1">
       <c r="B29" t="s">
         <v>28</v>
       </c>
@@ -1294,7 +1629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="2:6" outlineLevel="1">
+    <row r="30" spans="2:7" outlineLevel="1">
       <c r="B30" t="s">
         <v>29</v>
       </c>
@@ -1305,29 +1640,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="2:6" outlineLevel="1">
+    <row r="31" spans="2:7" outlineLevel="1">
       <c r="B31" t="s">
         <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="F31" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="2:6" outlineLevel="1">
+      <c r="G31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" outlineLevel="1">
       <c r="B32" t="s">
         <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="F32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" outlineLevel="1">
+      <c r="G32" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" outlineLevel="1">
       <c r="B33" t="s">
         <v>32</v>
       </c>
@@ -1338,7 +1679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" outlineLevel="1">
+    <row r="34" spans="1:7" outlineLevel="1">
       <c r="B34" t="s">
         <v>33</v>
       </c>
@@ -1349,7 +1690,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:6" outlineLevel="1">
+    <row r="35" spans="1:7" outlineLevel="1">
       <c r="B35" t="s">
         <v>34</v>
       </c>
@@ -1360,7 +1701,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:6" outlineLevel="1">
+    <row r="36" spans="1:7" outlineLevel="1">
       <c r="B36" t="s">
         <v>35</v>
       </c>
@@ -1371,7 +1712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" outlineLevel="1">
+    <row r="37" spans="1:7" outlineLevel="1">
       <c r="B37" t="s">
         <v>36</v>
       </c>
@@ -1382,7 +1723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:6" outlineLevel="1">
+    <row r="38" spans="1:7" outlineLevel="1">
       <c r="B38" t="s">
         <v>37</v>
       </c>
@@ -1393,7 +1734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:6" outlineLevel="1">
+    <row r="39" spans="1:7" outlineLevel="1">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -1404,7 +1745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:6" outlineLevel="1">
+    <row r="40" spans="1:7" outlineLevel="1">
       <c r="B40" t="s">
         <v>39</v>
       </c>
@@ -1415,7 +1756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:6" outlineLevel="1">
+    <row r="41" spans="1:7" outlineLevel="1">
       <c r="B41" t="s">
         <v>40</v>
       </c>
@@ -1426,7 +1767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" outlineLevel="1">
+    <row r="42" spans="1:7" outlineLevel="1">
       <c r="B42" t="s">
         <v>41</v>
       </c>
@@ -1437,7 +1778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:6" outlineLevel="1">
+    <row r="43" spans="1:7" outlineLevel="1">
       <c r="B43" t="s">
         <v>42</v>
       </c>
@@ -1448,31 +1789,31 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="14.25">
+    <row r="44" spans="1:7" ht="14.25">
       <c r="A44" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F44" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:6" outlineLevel="1">
+    <row r="45" spans="1:7" outlineLevel="1">
       <c r="B45" t="s">
+        <v>54</v>
+      </c>
+      <c r="E45" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" outlineLevel="1">
+      <c r="B46" t="s">
         <v>55</v>
-      </c>
-      <c r="E45" t="s">
-        <v>52</v>
-      </c>
-      <c r="F45" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" outlineLevel="1">
-      <c r="B46" t="s">
-        <v>56</v>
       </c>
       <c r="E46" t="s">
         <v>43</v>
@@ -1481,9 +1822,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:6" outlineLevel="1">
+    <row r="47" spans="1:7" outlineLevel="1">
       <c r="B47" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="E47" t="s">
         <v>43</v>
@@ -1491,55 +1832,61 @@
       <c r="F47" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" outlineLevel="1">
+      <c r="G47" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" outlineLevel="1">
       <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="E48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" outlineLevel="1">
+      <c r="B49" t="s">
+        <v>57</v>
+      </c>
+      <c r="E49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" outlineLevel="1">
+      <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" t="s">
+        <v>2</v>
+      </c>
+      <c r="G50" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" outlineLevel="1">
+      <c r="B51" t="s">
         <v>58</v>
       </c>
-      <c r="E48" t="s">
-        <v>52</v>
-      </c>
-      <c r="F48" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" outlineLevel="1">
-      <c r="B49" t="s">
+      <c r="E51" t="s">
+        <v>2</v>
+      </c>
+      <c r="F51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" outlineLevel="1">
+      <c r="B52" t="s">
         <v>59</v>
       </c>
-      <c r="E49" t="s">
-        <v>52</v>
-      </c>
-      <c r="F49" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" outlineLevel="1">
-      <c r="B50" t="s">
-        <v>60</v>
-      </c>
-      <c r="E50" t="s">
-        <v>2</v>
-      </c>
-      <c r="F50" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" outlineLevel="1">
-      <c r="B51" t="s">
-        <v>61</v>
-      </c>
-      <c r="E51" t="s">
-        <v>2</v>
-      </c>
-      <c r="F51" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" outlineLevel="1">
-      <c r="B52" t="s">
-        <v>65</v>
-      </c>
       <c r="E52" t="s">
         <v>2</v>
       </c>
@@ -1547,41 +1894,77 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:6" outlineLevel="1">
+    <row r="53" spans="2:7" outlineLevel="1">
       <c r="B53" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E53" t="s">
         <v>2</v>
       </c>
       <c r="F53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" outlineLevel="1">
+      <c r="B54" t="s">
+        <v>64</v>
+      </c>
+      <c r="E54" t="s">
+        <v>2</v>
+      </c>
+      <c r="F54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" outlineLevel="1">
+      <c r="B55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E55" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7">
+      <c r="E56" t="s">
+        <v>43</v>
+      </c>
+      <c r="F56" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="18" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+      <formula>"Invalid"</formula>
+    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E1:F1048576">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="equal">
+  <conditionalFormatting sqref="G47 E1:F1048576 G31:G32 G50">
+    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
       <formula>"NotStart"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
       <formula>"Processing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E82:E1048576">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E84:E1048576">
       <formula1>"NotStart,Processing,Complete"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E81 F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 E57:E83">
       <formula1>"NotStart,Processing,Completed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E56">
+      <formula1>"NotStart,Processing,Completed,Invalid"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1591,209 +1974,558 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:A39"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="1" max="1" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="28.375" customWidth="1"/>
+    <col min="3" max="3" width="40.875" customWidth="1"/>
+    <col min="4" max="4" width="52.125" customWidth="1"/>
+    <col min="5" max="5" width="34.875" customWidth="1"/>
+    <col min="6" max="6" width="18.625" customWidth="1"/>
+    <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
+    <row r="1" spans="1:7" ht="20.25">
+      <c r="A1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="14.25">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="27" outlineLevel="1">
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
+      <c r="C3" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="67.5" outlineLevel="1">
+      <c r="C4" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="27" outlineLevel="1">
+      <c r="C5" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="67.5" outlineLevel="1">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
+      <c r="C6" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="40.5" outlineLevel="1">
+      <c r="C7" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" outlineLevel="1">
+      <c r="C8" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" outlineLevel="1">
+      <c r="C9" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" outlineLevel="1">
+      <c r="B10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" outlineLevel="1">
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" outlineLevel="1">
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" outlineLevel="1">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
+      <c r="F13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" outlineLevel="1">
+      <c r="B14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" outlineLevel="1">
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" outlineLevel="1">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" outlineLevel="1">
+      <c r="B17" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
+      <c r="F17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" outlineLevel="1">
+      <c r="B18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" outlineLevel="1">
+      <c r="B19" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" outlineLevel="1">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
+      <c r="F20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" outlineLevel="1">
+      <c r="B21" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
+      <c r="F21" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" outlineLevel="1">
+      <c r="B22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="1:1">
-      <c r="A14" t="s">
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" outlineLevel="1">
+      <c r="B23" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" t="s">
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" outlineLevel="1">
+      <c r="B24" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" t="s">
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" outlineLevel="1">
+      <c r="B25" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" outlineLevel="1">
+      <c r="B26" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" outlineLevel="1">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" outlineLevel="1">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" outlineLevel="1">
+      <c r="B29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" outlineLevel="1">
+      <c r="B30" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" outlineLevel="1">
+      <c r="B31" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
+      <c r="F31" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" outlineLevel="1">
+      <c r="B32" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" outlineLevel="1">
+      <c r="B33" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
+      <c r="F33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" outlineLevel="1">
+      <c r="B34" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
+      <c r="F34" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" outlineLevel="1">
+      <c r="B35" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
+      <c r="F35" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" outlineLevel="1">
+      <c r="B36" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" outlineLevel="1">
+      <c r="B37" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
+      <c r="F37" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" outlineLevel="1">
+      <c r="B38" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
+      <c r="F38" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" outlineLevel="1">
+      <c r="B39" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
+      <c r="F39" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" outlineLevel="1">
+      <c r="B40" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
+      <c r="F40" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" outlineLevel="1">
+      <c r="B41" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+      <c r="F41" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" outlineLevel="1">
+      <c r="B42" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
+      <c r="F42" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" outlineLevel="1">
+      <c r="B43" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
+      <c r="F43" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" outlineLevel="1">
+      <c r="B44" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
+      <c r="F44" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" outlineLevel="1">
+      <c r="B45" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
+      <c r="F45" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" outlineLevel="1">
+      <c r="B46" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
+      <c r="F46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" outlineLevel="1">
+      <c r="B47" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
+      <c r="F47" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" outlineLevel="1">
+      <c r="B48" t="s">
         <v>42</v>
+      </c>
+      <c r="F48" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="14.25">
+      <c r="A49" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" outlineLevel="1">
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="F50" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" outlineLevel="1">
+      <c r="B51" t="s">
+        <v>55</v>
+      </c>
+      <c r="F51" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" outlineLevel="1">
+      <c r="B52" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" outlineLevel="1">
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+      <c r="F53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" outlineLevel="1">
+      <c r="B54" t="s">
+        <v>57</v>
+      </c>
+      <c r="F54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" outlineLevel="1">
+      <c r="B55" t="s">
+        <v>72</v>
+      </c>
+      <c r="F55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" outlineLevel="1">
+      <c r="B56" t="s">
+        <v>58</v>
+      </c>
+      <c r="F56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" outlineLevel="1">
+      <c r="B57" t="s">
+        <v>59</v>
+      </c>
+      <c r="F57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" outlineLevel="1">
+      <c r="B58" t="s">
+        <v>63</v>
+      </c>
+      <c r="F58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" outlineLevel="1">
+      <c r="B59" t="s">
+        <v>64</v>
+      </c>
+      <c r="F59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" outlineLevel="1">
+      <c r="B60" t="s">
+        <v>71</v>
+      </c>
+      <c r="F60" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="G52 G36:G37 G55 F1:F60">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+      <formula>"NotStart"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+      <formula>"Processing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F1:F60">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+      <formula>"Invalid"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Completed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F60">
+      <formula1>"NotStart,Processing,Completed,Invalid"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Try to solve double handle release, but there still an unknown bug... Signed-off-by: Gene Kong <gyx_edu@qq.com>
</commit_message>
<xml_diff>
--- a/schedule/Project Track.xlsx
+++ b/schedule/Project Track.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Port Plan" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="89">
   <si>
     <t>Decription</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -444,6 +444,10 @@
   </si>
   <si>
     <t>Test Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RemoveCb</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -647,77 +651,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -777,13 +711,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
@@ -791,161 +718,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF339933"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1246,11 +1019,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -1446,6 +1219,9 @@
       <c r="B13" t="s">
         <v>12</v>
       </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
       <c r="E13" t="s">
         <v>43</v>
       </c>
@@ -1938,21 +1714,21 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"Invalid"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47 E1:F1048576 G31:G32 G50">
-    <cfRule type="cellIs" dxfId="36" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>"NotStart"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="equal">
       <formula>"Processing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1976,11 +1752,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -2503,21 +2279,21 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="G52 G36:G37 G55 F1:F60">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"NotStart"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Processing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F60">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
       <formula>"Invalid"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Review and update fixed some bug.
Signed-off-by: Gene Kong <gyx_edu@qq.com>
</commit_message>
<xml_diff>
--- a/schedule/Project Track.xlsx
+++ b/schedule/Project Track.xlsx
@@ -1023,7 +1023,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D51" sqref="D51"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -1289,7 +1289,7 @@
         <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F19" t="s">
         <v>2</v>
@@ -1300,7 +1300,7 @@
         <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
update some function and chinese documnet.
</commit_message>
<xml_diff>
--- a/schedule/Project Track.xlsx
+++ b/schedule/Project Track.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="91">
   <si>
     <t>Decription</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -448,6 +448,14 @@
   </si>
   <si>
     <t>RemoveCb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Diffcult to port.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Invalid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1023,7 +1031,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A20" sqref="A20:XFD20"/>
+      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -1124,6 +1132,9 @@
       <c r="C6" t="s">
         <v>51</v>
       </c>
+      <c r="D6" t="s">
+        <v>89</v>
+      </c>
       <c r="E6" t="s">
         <v>2</v>
       </c>
@@ -1233,6 +1244,9 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
+      <c r="D14" t="s">
+        <v>90</v>
+      </c>
       <c r="E14" t="s">
         <v>43</v>
       </c>
@@ -1460,7 +1474,7 @@
         <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
         <v>2</v>
@@ -1471,7 +1485,7 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>2</v>
+        <v>77</v>
       </c>
       <c r="F35" t="s">
         <v>2</v>
@@ -1504,7 +1518,7 @@
         <v>37</v>
       </c>
       <c r="E38" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="F38" t="s">
         <v>2</v>

</xml_diff>